<commit_message>
Hoàn thành chức năng xem chi tiết sản phẩm, thêm sản phẩm vào hóa đơn, gửi xác nhận tới cửa hàng. Hoàn thành tạo csdl cục bộ ở điện thoại
</commit_message>
<xml_diff>
--- a/KLTN/Tiến độ/Android.xlsx
+++ b/KLTN/Tiến độ/Android.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Thời gian</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Lê Thanh Tuấn</t>
   </si>
   <si>
-    <t>30/1/2018</t>
-  </si>
-  <si>
     <t>Công việc thực hiện được</t>
   </si>
   <si>
@@ -73,6 +70,22 @@
   </si>
   <si>
     <t>22/1/2018 - 3/2/2018</t>
+  </si>
+  <si>
+    <t>30/1/2018 - 9/2/2018</t>
+  </si>
+  <si>
+    <t>Hoàn thành giao diện đăng nhập
+Hoàn thành giao diện trang sản phẩm
+Hoàn thành giao diện danh mục sản phẩm cần mua
+Tìm được dữ liệu mẫu cho ứng dụng
+Hoàn thành chức năng đăng nhập
+Hoàn thành chức năng thêm sản phẩm vào danh mục sản phẩm cần mua
+Hoàn thành chức năng xác nhận danh mục sản phẩm cần mua
+Hoàn thành chức năng xem sản phẩm</t>
+  </si>
+  <si>
+    <t>Trễ 5 ngày so với tiến độ</t>
   </si>
 </sst>
 </file>
@@ -96,7 +109,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -154,11 +167,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -166,14 +205,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,7 +527,7 @@
   <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,76 +548,76 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4" t="s">
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -583,161 +632,171 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.140625" customWidth="1"/>
+    <col min="4" max="4" width="55.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+    <row r="3" spans="1:6" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>